<commit_message>
updated word doc for patux redux, need to proof
</commit_message>
<xml_diff>
--- a/word/Tables.xlsx
+++ b/word/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Table 5" sheetId="5" r:id="rId5"/>
     <sheet name="Table 6" sheetId="6" r:id="rId6"/>
     <sheet name="Table 7" sheetId="7" r:id="rId7"/>
+    <sheet name="Table 8" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="142">
   <si>
     <t>Station</t>
   </si>
@@ -836,6 +837,95 @@
   </si>
   <si>
     <r>
+      <t>TABLE 4: Summaries of flow-normalized  trends from each model  at TF1.6 for different time periods. Summaries  are averages and percentage changes of ln-chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>g/L ) based on annual means within each category.  For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
+    </r>
+  </si>
+  <si>
+    <t>Add hats to second chl text in each formula</t>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 3: Summaries of flow-normalized trends from each model at LE1.2 for different time periods. Summaries are averages and percentage changes of ln-chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>g/L) based on annual means within each category. For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Chl</t>
     </r>
     <r>
@@ -845,7 +935,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-        <family val="1"/>
       </rPr>
       <t>obs</t>
     </r>
@@ -866,106 +955,133 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-        <family val="1"/>
       </rPr>
       <t>obs</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>TABLE 4: Summaries of flow-normalized  trends from each model  at TF1.6 for different time periods. Summaries  are averages and percentage changes of ln-chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>g/L ) based on annual means within each category.  For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
-    </r>
-  </si>
-  <si>
-    <t>Add hats to second chl text in each formula</t>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 3: Summaries of flow-normalized trends from each model at LE1.2 for different time periods. Summaries are averages and percentage changes of ln-chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>g/L) based on annual means within each category. For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
-    </r>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>ease of use</t>
+  </si>
+  <si>
+    <t>computational requirements</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>visualization</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>statistical</t>
+  </si>
+  <si>
+    <t>additional variables</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>censored data</t>
+  </si>
+  <si>
+    <t>confidence intervals</t>
+  </si>
+  <si>
+    <t>quantile fits</t>
+  </si>
+  <si>
+    <r>
+      <t>interpretation</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>software and documentation</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Relates to statistical foundation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>In reference to analysis of water quality trends</t>
+    </r>
+  </si>
+  <si>
+    <t>TABLE 8: Qualitative comparisons of generalized additive models and WRTDS. Qualities are grouped by ease of use and statistical considerations. Ease of use qualities are described as good, moderate, or poor and statistical qualities as yes/no.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1028,6 +1144,39 @@
       <name val="Times"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1078,7 +1227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1100,9 +1249,6 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1188,15 +1334,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1252,6 +1389,44 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1552,40 +1727,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="67" t="s">
         <v>109</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="H2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1593,25 +1768,25 @@
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="35">
         <v>38.81</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="35">
         <v>-76.709999999999994</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="36">
+      <c r="E3" s="35">
         <v>74.900000000000006</v>
       </c>
-      <c r="F3" s="36">
+      <c r="F3" s="35">
         <v>2.9</v>
       </c>
-      <c r="G3" s="36">
+      <c r="G3" s="35">
         <v>1.52</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="35">
         <v>0</v>
       </c>
     </row>
@@ -1619,25 +1794,25 @@
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="36">
+      <c r="B4" s="35">
         <v>38.770000000000003</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="35">
         <v>-76.709999999999994</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="36">
+      <c r="E4" s="35">
         <v>69.5</v>
       </c>
-      <c r="F4" s="36">
+      <c r="F4" s="35">
         <v>2</v>
       </c>
-      <c r="G4" s="36">
+      <c r="G4" s="35">
         <v>2.31</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="35">
         <v>0.02</v>
       </c>
     </row>
@@ -1645,25 +1820,25 @@
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="36">
+      <c r="B5" s="35">
         <v>38.71</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <v>-76.7</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="36">
+      <c r="E5" s="35">
         <v>60.3</v>
       </c>
-      <c r="F5" s="36">
+      <c r="F5" s="35">
         <v>10.6</v>
       </c>
-      <c r="G5" s="36">
+      <c r="G5" s="35">
         <v>2.88</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="35">
         <v>0.27</v>
       </c>
     </row>
@@ -1671,25 +1846,25 @@
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="35">
         <v>38.659999999999997</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <v>-76.680000000000007</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="36">
+      <c r="E6" s="35">
         <v>52.2</v>
       </c>
-      <c r="F6" s="36">
+      <c r="F6" s="35">
         <v>6.2</v>
       </c>
-      <c r="G6" s="36">
+      <c r="G6" s="35">
         <v>2.44</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="35">
         <v>0.9</v>
       </c>
     </row>
@@ -1697,25 +1872,25 @@
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="35">
         <v>38.58</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>-76.680000000000007</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="36">
+      <c r="E7" s="35">
         <v>42.5</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="35">
         <v>3</v>
       </c>
-      <c r="G7" s="36">
+      <c r="G7" s="35">
         <v>2.09</v>
       </c>
-      <c r="H7" s="36">
+      <c r="H7" s="35">
         <v>4.09</v>
       </c>
     </row>
@@ -1723,25 +1898,25 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="35">
         <v>38.49</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>-76.66</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="36">
+      <c r="E8" s="35">
         <v>32.200000000000003</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>11.2</v>
       </c>
-      <c r="G8" s="36">
+      <c r="G8" s="35">
         <v>2.4700000000000002</v>
       </c>
-      <c r="H8" s="36">
+      <c r="H8" s="35">
         <v>10.25</v>
       </c>
     </row>
@@ -1749,25 +1924,25 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="35">
         <v>38.43</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <v>-76.599999999999994</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="36">
+      <c r="E9" s="35">
         <v>22.9</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="35">
         <v>12.1</v>
       </c>
-      <c r="G9" s="36">
+      <c r="G9" s="35">
         <v>2.31</v>
       </c>
-      <c r="H9" s="36">
+      <c r="H9" s="35">
         <v>12.04</v>
       </c>
     </row>
@@ -1775,25 +1950,25 @@
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="36">
+      <c r="B10" s="35">
         <v>38.380000000000003</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <v>-76.510000000000005</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="36">
+      <c r="E10" s="35">
         <v>13.4</v>
       </c>
-      <c r="F10" s="36">
+      <c r="F10" s="35">
         <v>17.100000000000001</v>
       </c>
-      <c r="G10" s="36">
+      <c r="G10" s="35">
         <v>2.16</v>
       </c>
-      <c r="H10" s="36">
+      <c r="H10" s="35">
         <v>12.73</v>
       </c>
     </row>
@@ -1801,25 +1976,25 @@
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="36">
+      <c r="B11" s="35">
         <v>38.340000000000003</v>
       </c>
-      <c r="C11" s="36">
+      <c r="C11" s="35">
         <v>-76.48</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="36">
+      <c r="E11" s="35">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F11" s="36">
+      <c r="F11" s="35">
         <v>23.4</v>
       </c>
-      <c r="G11" s="36">
+      <c r="G11" s="35">
         <v>2.12</v>
       </c>
-      <c r="H11" s="36">
+      <c r="H11" s="35">
         <v>12.89</v>
       </c>
     </row>
@@ -1827,25 +2002,25 @@
       <c r="A12" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="36">
         <v>38.31</v>
       </c>
-      <c r="C12" s="37">
+      <c r="C12" s="36">
         <v>-76.42</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E12" s="37">
+      <c r="E12" s="36">
         <v>0</v>
       </c>
-      <c r="F12" s="37">
+      <c r="F12" s="36">
         <v>15.4</v>
       </c>
-      <c r="G12" s="37">
+      <c r="G12" s="36">
         <v>2.21</v>
       </c>
-      <c r="H12" s="37">
+      <c r="H12" s="36">
         <v>13.46</v>
       </c>
     </row>
@@ -1876,67 +2051,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="C2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="25"/>
+      <c r="F2" s="24"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="14" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="5"/>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="13"/>
+      <c r="D4" s="12"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="9" t="s">
+      <c r="A5" s="15"/>
+      <c r="B5" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1944,27 +2119,27 @@
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1972,17 +2147,17 @@
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10" t="s">
+      <c r="D8" s="9"/>
+      <c r="E8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1990,35 +2165,35 @@
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10" t="s">
+      <c r="D9" s="9"/>
+      <c r="E9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>48</v>
       </c>
     </row>
@@ -2026,27 +2201,27 @@
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2054,17 +2229,17 @@
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10" t="s">
+      <c r="D13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2072,117 +2247,117 @@
       <c r="A14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10" t="s">
+      <c r="D14" s="9"/>
+      <c r="E14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C15" s="9" t="s">
+      <c r="C15" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="9" t="s">
+      <c r="F15" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
+      <c r="B16" s="9"/>
+      <c r="C16" s="9"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="9"/>
+      <c r="E17" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="9"/>
+      <c r="E18" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>3</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="9"/>
+      <c r="E19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F20" s="8" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2217,28 +2392,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="53" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="56" t="s">
+      <c r="C2" s="52"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="56"/>
+      <c r="F2" s="52"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -2257,28 +2432,28 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="68"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="37">
+      <c r="A5" s="23"/>
+      <c r="B5" s="36">
         <v>2.17</v>
       </c>
-      <c r="C5" s="37">
+      <c r="C5" s="36">
         <v>24.28</v>
       </c>
-      <c r="D5" s="40"/>
-      <c r="E5" s="37">
+      <c r="D5" s="69"/>
+      <c r="E5" s="36">
         <v>2.1800000000000002</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="36">
         <v>18.850000000000001</v>
       </c>
     </row>
@@ -2286,27 +2461,27 @@
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="36">
+      <c r="B7" s="35">
         <v>1.99</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>9.6</v>
       </c>
-      <c r="D7" s="41"/>
-      <c r="E7" s="36">
+      <c r="D7" s="70"/>
+      <c r="E7" s="35">
         <v>2.0299999999999998</v>
       </c>
-      <c r="F7" s="36">
+      <c r="F7" s="35">
         <v>1.75</v>
       </c>
     </row>
@@ -2314,17 +2489,17 @@
       <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="36">
+      <c r="B8" s="35">
         <v>2.12</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <v>5.49</v>
       </c>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36">
+      <c r="D8" s="35"/>
+      <c r="E8" s="35">
         <v>2.12</v>
       </c>
-      <c r="F8" s="36">
+      <c r="F8" s="35">
         <v>5.5</v>
       </c>
     </row>
@@ -2332,63 +2507,63 @@
       <c r="A9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="36">
+      <c r="B9" s="35">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C9" s="35">
         <v>5.5</v>
       </c>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36">
+      <c r="D9" s="35"/>
+      <c r="E9" s="35">
         <v>2.2400000000000002</v>
       </c>
-      <c r="F9" s="36">
+      <c r="F9" s="35">
         <v>5.35</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="37">
+      <c r="B10" s="36">
         <v>2.37</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="36">
         <v>3.2</v>
       </c>
-      <c r="D10" s="37"/>
-      <c r="E10" s="37">
+      <c r="D10" s="36"/>
+      <c r="E10" s="36">
         <v>2.37</v>
       </c>
-      <c r="F10" s="37">
+      <c r="F10" s="36">
         <v>6.07</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="39"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="35"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="35"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="35">
         <v>2.57</v>
       </c>
-      <c r="C12" s="36">
+      <c r="C12" s="35">
         <v>20.059999999999999</v>
       </c>
-      <c r="D12" s="41"/>
-      <c r="E12" s="36">
+      <c r="D12" s="70"/>
+      <c r="E12" s="35">
         <v>2.58</v>
       </c>
-      <c r="F12" s="36">
+      <c r="F12" s="35">
         <v>14.04</v>
       </c>
     </row>
@@ -2396,17 +2571,17 @@
       <c r="A13" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="36">
+      <c r="B13" s="35">
         <v>2.3199999999999998</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="35">
         <v>31.2</v>
       </c>
-      <c r="D13" s="36"/>
-      <c r="E13" s="36">
+      <c r="D13" s="35"/>
+      <c r="E13" s="35">
         <v>2.33</v>
       </c>
-      <c r="F13" s="36">
+      <c r="F13" s="35">
         <v>22.47</v>
       </c>
     </row>
@@ -2414,35 +2589,35 @@
       <c r="A14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="35">
         <v>2.0099999999999998</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="35">
         <v>18.48</v>
       </c>
-      <c r="D14" s="36"/>
-      <c r="E14" s="36">
+      <c r="D14" s="35"/>
+      <c r="E14" s="35">
         <v>2.0099999999999998</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="35">
         <v>19.91</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="37">
+      <c r="B15" s="36">
         <v>1.82</v>
       </c>
-      <c r="C15" s="37">
+      <c r="C15" s="36">
         <v>25.29</v>
       </c>
-      <c r="D15" s="37"/>
-      <c r="E15" s="37">
+      <c r="D15" s="36"/>
+      <c r="E15" s="36">
         <v>1.83</v>
       </c>
-      <c r="F15" s="37">
+      <c r="F15" s="36">
         <v>15.14</v>
       </c>
     </row>
@@ -2450,81 +2625,81 @@
       <c r="A16" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="36"/>
-      <c r="C16" s="36"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="36">
+      <c r="B17" s="35">
         <v>1.9</v>
       </c>
-      <c r="C17" s="36">
+      <c r="C17" s="35">
         <v>20.86</v>
       </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="36">
+      <c r="D17" s="70"/>
+      <c r="E17" s="35">
         <v>1.93</v>
       </c>
-      <c r="F17" s="36">
+      <c r="F17" s="35">
         <v>16.77</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="36">
+      <c r="B18" s="35">
         <v>2.1</v>
       </c>
-      <c r="C18" s="36">
+      <c r="C18" s="35">
         <v>13.71</v>
       </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36">
+      <c r="D18" s="35"/>
+      <c r="E18" s="35">
         <v>2.11</v>
       </c>
-      <c r="F18" s="36">
+      <c r="F18" s="35">
         <v>7.73</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="18">
         <v>3</v>
       </c>
-      <c r="B19" s="36">
+      <c r="B19" s="35">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C19" s="36">
+      <c r="C19" s="35">
         <v>15.66</v>
       </c>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36">
+      <c r="D19" s="35"/>
+      <c r="E19" s="35">
         <v>2.29</v>
       </c>
-      <c r="F19" s="36">
+      <c r="F19" s="35">
         <v>9.24</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="36">
         <v>2.34</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="36">
         <v>25.09</v>
       </c>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37">
+      <c r="D20" s="36"/>
+      <c r="E20" s="36">
         <v>2.33</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="36">
         <v>22.29</v>
       </c>
     </row>
@@ -2550,40 +2725,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5703125" style="26" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="26"/>
-    <col min="3" max="3" width="11.140625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" style="26" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="26"/>
-    <col min="6" max="6" width="10.7109375" style="26" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="13.5703125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="25"/>
+    <col min="3" max="3" width="11.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="3.140625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="25"/>
+    <col min="6" max="6" width="10.7109375" style="25" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="A1" s="67" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="47" t="s">
+      <c r="A2" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="C2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="53"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="7" t="s">
         <v>89</v>
       </c>
@@ -2599,274 +2774,274 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
-      <c r="B5" s="32">
+      <c r="A5" s="51"/>
+      <c r="B5" s="31">
         <v>2.4300000000000002</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>-4.8099999999999996</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31">
         <v>2.44</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="31">
         <v>-2.2799999999999998</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>2.62</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>-4.93</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32">
         <v>2.6</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>-3.06</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>2.69</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>-5.05</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32">
         <v>2.65</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>-3.55</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>2.15</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>-22.42</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32">
         <v>2.19</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>-21.51</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>2.2400000000000002</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>47.1</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32">
+      <c r="D10" s="31"/>
+      <c r="E10" s="31">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>38.35</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="31"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>1.52</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>9.0299999999999994</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32">
         <v>1.48</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <v>32.72</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>2.63</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>5.47</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32">
         <v>2.62</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>5.14</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>3.06</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>0.04</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33">
+      <c r="D14" s="32"/>
+      <c r="E14" s="32">
         <v>3.08</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>0.79</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>2.17</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>-18.16</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="31">
         <v>-17.55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>2.89</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="32">
         <v>-4.78</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33">
+      <c r="D17" s="32"/>
+      <c r="E17" s="32">
         <v>2.93</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <v>-0.42</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="25">
         <v>2</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>2.41</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="32">
         <v>16.71</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33">
+      <c r="D18" s="32"/>
+      <c r="E18" s="32">
         <v>2.4300000000000002</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <v>20.309999999999999</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
+      <c r="A19" s="25">
         <v>3</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>2.2799999999999998</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="32">
         <v>6.53</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33">
+      <c r="D19" s="32"/>
+      <c r="E19" s="32">
         <v>2.27</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <v>15.2</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>2.2200000000000002</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>-11.58</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32">
+      <c r="D20" s="31"/>
+      <c r="E20" s="31">
         <v>2.21</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <v>-11.27</v>
       </c>
     </row>
@@ -2896,28 +3071,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="67" t="s">
         <v>111</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="59" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="59"/>
+      <c r="F2" s="55"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -2936,274 +3111,274 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="24"/>
-      <c r="B5" s="32">
+      <c r="A5" s="23"/>
+      <c r="B5" s="31">
         <v>-0.11</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="31">
         <v>0.09</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="32">
+      <c r="D5" s="31"/>
+      <c r="E5" s="31">
         <v>0.01</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="31">
         <v>0.13</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>0.2</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>0.1</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32">
         <v>-0.74</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>0.11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>0.34</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>0.09</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32">
         <v>-1.29</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>0.15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>-0.55000000000000004</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33">
+      <c r="D9" s="32"/>
+      <c r="E9" s="32">
         <v>0.68</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>0.13</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="27" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>-0.53</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>0.08</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32">
+      <c r="D10" s="31"/>
+      <c r="E10" s="31">
         <v>3.1</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>0.39</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>0.12</v>
       </c>
-      <c r="D12" s="35"/>
-      <c r="E12" s="33">
+      <c r="D12" s="34"/>
+      <c r="E12" s="32">
         <v>-2</v>
       </c>
-      <c r="F12" s="33">
+      <c r="F12" s="32">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>0.22</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>0.1</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="33">
+      <c r="D13" s="32"/>
+      <c r="E13" s="32">
         <v>-0.66</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>-0.71</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>0.06</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="33">
+      <c r="D14" s="32"/>
+      <c r="E14" s="32">
         <v>0.76</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>0.1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>-0.46</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>0.05</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="32">
+      <c r="D15" s="31"/>
+      <c r="E15" s="31">
         <v>1.04</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="31">
         <v>0.15</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
+      <c r="A16" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="33">
+      <c r="B17" s="32">
         <v>-0.27</v>
       </c>
-      <c r="C17" s="33">
+      <c r="C17" s="32">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="D17" s="35"/>
-      <c r="E17" s="33">
+      <c r="D17" s="34"/>
+      <c r="E17" s="32">
         <v>-0.15</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <v>0.1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="25">
         <v>2</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>-0.14000000000000001</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="32">
         <v>0.09</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33">
+      <c r="D18" s="32"/>
+      <c r="E18" s="32">
         <v>0.7</v>
       </c>
-      <c r="F18" s="33">
+      <c r="F18" s="32">
         <v>0.13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
+      <c r="A19" s="25">
         <v>3</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>0.49</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="32">
         <v>0.11</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="33">
+      <c r="D19" s="32"/>
+      <c r="E19" s="32">
         <v>1.07</v>
       </c>
-      <c r="F19" s="33">
+      <c r="F19" s="32">
         <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>-0.53</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="31">
         <v>0.09</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32">
+      <c r="D20" s="31"/>
+      <c r="E20" s="31">
         <v>-1.75</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="31">
         <v>0.15</v>
       </c>
     </row>
@@ -3236,550 +3411,550 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="67"/>
+      <c r="I1" s="67"/>
+      <c r="J1" s="67"/>
+      <c r="K1" s="67"/>
+      <c r="L1" s="67"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="59" t="s">
+      <c r="C2" s="55"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="59"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="59" t="s">
+      <c r="F2" s="55"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="59"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="59" t="s">
+      <c r="I2" s="55"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="59"/>
+      <c r="L2" s="55"/>
     </row>
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="38" t="s">
         <v>113</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="38" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="42" t="s">
+      <c r="F3" s="38" t="s">
         <v>113</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="42" t="s">
+      <c r="H3" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="38" t="s">
         <v>115</v>
       </c>
       <c r="J3" s="6"/>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="38" t="s">
         <v>114</v>
       </c>
-      <c r="L3" s="42" t="s">
+      <c r="L3" s="38" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="39"/>
+      <c r="I4" s="39"/>
+      <c r="J4" s="39"/>
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="61"/>
-      <c r="B5" s="44">
+      <c r="A5" s="57"/>
+      <c r="B5" s="40">
         <v>0.05</v>
       </c>
-      <c r="C5" s="44">
+      <c r="C5" s="40">
         <v>0.97</v>
       </c>
-      <c r="D5" s="32"/>
-      <c r="E5" s="44">
+      <c r="D5" s="31"/>
+      <c r="E5" s="40">
         <v>0.08</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="40">
         <v>0.97</v>
       </c>
-      <c r="G5" s="32"/>
-      <c r="H5" s="44">
+      <c r="G5" s="31"/>
+      <c r="H5" s="40">
         <v>0.15</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="40">
         <v>0.94</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32">
+      <c r="J5" s="31"/>
+      <c r="K5" s="31">
         <v>0.02</v>
       </c>
-      <c r="L5" s="32">
+      <c r="L5" s="31">
         <v>0.99</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="45" t="s">
+      <c r="A6" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="31"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="B6" s="32"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="30"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="26" t="s">
+      <c r="A7" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>0.02</v>
       </c>
-      <c r="C7" s="33">
+      <c r="C7" s="32">
         <v>0.99</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33">
+      <c r="D7" s="32"/>
+      <c r="E7" s="32">
         <v>-0.02</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>1</v>
       </c>
-      <c r="G7" s="33"/>
-      <c r="H7" s="46">
+      <c r="G7" s="32"/>
+      <c r="H7" s="42">
         <v>0.2</v>
       </c>
-      <c r="I7" s="46">
+      <c r="I7" s="42">
         <v>0.92</v>
       </c>
-      <c r="J7" s="33"/>
-      <c r="K7" s="46">
+      <c r="J7" s="32"/>
+      <c r="K7" s="42">
         <v>-0.12</v>
       </c>
-      <c r="L7" s="46">
+      <c r="L7" s="42">
         <v>1.03</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="26" t="s">
+      <c r="A8" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="46">
+      <c r="B8" s="42">
         <v>0.16</v>
       </c>
-      <c r="C8" s="46">
+      <c r="C8" s="42">
         <v>0.93</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33">
+      <c r="D8" s="32"/>
+      <c r="E8" s="32">
         <v>-0.03</v>
       </c>
-      <c r="F8" s="33">
+      <c r="F8" s="32">
         <v>0.99</v>
       </c>
-      <c r="G8" s="33"/>
-      <c r="H8" s="46">
+      <c r="G8" s="32"/>
+      <c r="H8" s="42">
         <v>0.17</v>
       </c>
-      <c r="I8" s="46">
+      <c r="I8" s="42">
         <v>0.92</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="46">
+      <c r="J8" s="32"/>
+      <c r="K8" s="42">
         <v>-0.12</v>
       </c>
-      <c r="L8" s="46">
+      <c r="L8" s="42">
         <v>1.02</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>0.02</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>0.99</v>
       </c>
-      <c r="D9" s="33"/>
-      <c r="E9" s="46">
+      <c r="D9" s="32"/>
+      <c r="E9" s="42">
         <v>0.13</v>
       </c>
-      <c r="F9" s="46">
+      <c r="F9" s="42">
         <v>0.95</v>
       </c>
-      <c r="G9" s="33"/>
-      <c r="H9" s="46">
+      <c r="G9" s="32"/>
+      <c r="H9" s="42">
         <v>0.06</v>
       </c>
-      <c r="I9" s="46">
+      <c r="I9" s="42">
         <v>0.98</v>
       </c>
-      <c r="J9" s="33"/>
-      <c r="K9" s="46">
+      <c r="J9" s="32"/>
+      <c r="K9" s="42">
         <v>0.11</v>
       </c>
-      <c r="L9" s="46">
+      <c r="L9" s="42">
         <v>0.97</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="32">
+      <c r="B10" s="31">
         <v>0</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="31">
         <v>1</v>
       </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="44">
+      <c r="D10" s="31"/>
+      <c r="E10" s="40">
         <v>0.12</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="31">
         <v>0.97</v>
       </c>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32">
+      <c r="G10" s="31"/>
+      <c r="H10" s="31">
         <v>0.01</v>
       </c>
-      <c r="I10" s="32">
+      <c r="I10" s="31">
         <v>0.99</v>
       </c>
-      <c r="J10" s="32"/>
-      <c r="K10" s="44">
+      <c r="J10" s="31"/>
+      <c r="K10" s="40">
         <v>0.08</v>
       </c>
-      <c r="L10" s="32">
+      <c r="L10" s="31">
         <v>0.99</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="33"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
-      <c r="L11" s="33"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+      <c r="L11" s="32"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="26" t="s">
+      <c r="A12" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>-0.01</v>
       </c>
-      <c r="C12" s="33">
+      <c r="C12" s="32">
         <v>1.01</v>
       </c>
-      <c r="D12" s="33"/>
-      <c r="E12" s="33">
+      <c r="D12" s="32"/>
+      <c r="E12" s="32">
         <v>0.09</v>
       </c>
-      <c r="F12" s="46">
+      <c r="F12" s="42">
         <v>0.92</v>
       </c>
-      <c r="G12" s="33"/>
-      <c r="H12" s="33">
+      <c r="G12" s="32"/>
+      <c r="H12" s="32">
         <v>0.01</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="32">
         <v>1</v>
       </c>
-      <c r="J12" s="33"/>
-      <c r="K12" s="46">
+      <c r="J12" s="32"/>
+      <c r="K12" s="42">
         <v>0.2</v>
       </c>
-      <c r="L12" s="46">
+      <c r="L12" s="42">
         <v>0.84</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="26" t="s">
+      <c r="A13" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="46">
+      <c r="B13" s="42">
         <v>0.28000000000000003</v>
       </c>
-      <c r="C13" s="46">
+      <c r="C13" s="42">
         <v>0.88</v>
       </c>
-      <c r="D13" s="33"/>
-      <c r="E13" s="46">
+      <c r="D13" s="32"/>
+      <c r="E13" s="42">
         <v>0.27</v>
       </c>
-      <c r="F13" s="46">
+      <c r="F13" s="42">
         <v>0.89</v>
       </c>
-      <c r="G13" s="33"/>
-      <c r="H13" s="46">
+      <c r="G13" s="32"/>
+      <c r="H13" s="42">
         <v>0.38</v>
       </c>
-      <c r="I13" s="46">
+      <c r="I13" s="42">
         <v>0.84</v>
       </c>
-      <c r="J13" s="33"/>
-      <c r="K13" s="46">
+      <c r="J13" s="32"/>
+      <c r="K13" s="42">
         <v>0.34</v>
       </c>
-      <c r="L13" s="46">
+      <c r="L13" s="42">
         <v>0.87</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="26" t="s">
+      <c r="A14" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>-0.08</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>1.03</v>
       </c>
-      <c r="D14" s="33"/>
-      <c r="E14" s="46">
+      <c r="D14" s="32"/>
+      <c r="E14" s="42">
         <v>0.34</v>
       </c>
-      <c r="F14" s="46">
+      <c r="F14" s="42">
         <v>0.89</v>
       </c>
-      <c r="G14" s="33"/>
-      <c r="H14" s="46">
+      <c r="G14" s="32"/>
+      <c r="H14" s="42">
         <v>0.3</v>
       </c>
-      <c r="I14" s="46">
+      <c r="I14" s="42">
         <v>0.85</v>
       </c>
-      <c r="J14" s="33"/>
-      <c r="K14" s="46">
+      <c r="J14" s="32"/>
+      <c r="K14" s="42">
         <v>0.39</v>
       </c>
-      <c r="L14" s="46">
+      <c r="L14" s="42">
         <v>0.88</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="32">
+      <c r="B15" s="31">
         <v>0.02</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="31">
         <v>0.98</v>
       </c>
-      <c r="D15" s="32"/>
-      <c r="E15" s="44">
+      <c r="D15" s="31"/>
+      <c r="E15" s="40">
         <v>0.13</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="40">
         <v>0.95</v>
       </c>
-      <c r="G15" s="32"/>
-      <c r="H15" s="44">
+      <c r="G15" s="31"/>
+      <c r="H15" s="40">
         <v>0.38</v>
       </c>
-      <c r="I15" s="44">
+      <c r="I15" s="40">
         <v>0.8</v>
       </c>
-      <c r="J15" s="32"/>
-      <c r="K15" s="32">
+      <c r="J15" s="31"/>
+      <c r="K15" s="31">
         <v>0.03</v>
       </c>
-      <c r="L15" s="32">
+      <c r="L15" s="31">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="43" t="s">
         <v>70</v>
       </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="33"/>
-      <c r="G16" s="33"/>
-      <c r="H16" s="33"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="33"/>
-      <c r="K16" s="33"/>
-      <c r="L16" s="33"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="32"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="46">
+      <c r="B17" s="42">
         <v>0.14000000000000001</v>
       </c>
-      <c r="C17" s="46">
+      <c r="C17" s="42">
         <v>0.92</v>
       </c>
-      <c r="D17" s="33"/>
-      <c r="E17" s="33">
+      <c r="D17" s="32"/>
+      <c r="E17" s="32">
         <v>-0.03</v>
       </c>
-      <c r="F17" s="33">
+      <c r="F17" s="32">
         <v>1.01</v>
       </c>
-      <c r="G17" s="33"/>
-      <c r="H17" s="46">
+      <c r="G17" s="32"/>
+      <c r="H17" s="42">
         <v>0.46</v>
       </c>
-      <c r="I17" s="46">
+      <c r="I17" s="42">
         <v>0.77</v>
       </c>
-      <c r="J17" s="33"/>
-      <c r="K17" s="46">
+      <c r="J17" s="32"/>
+      <c r="K17" s="42">
         <v>0.16</v>
       </c>
-      <c r="L17" s="46">
+      <c r="L17" s="42">
         <v>0.95</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="26">
+      <c r="A18" s="25">
         <v>2</v>
       </c>
-      <c r="B18" s="33">
+      <c r="B18" s="32">
         <v>0</v>
       </c>
-      <c r="C18" s="33">
+      <c r="C18" s="32">
         <v>1</v>
       </c>
-      <c r="D18" s="33"/>
-      <c r="E18" s="46">
+      <c r="D18" s="32"/>
+      <c r="E18" s="42">
         <v>0.12</v>
       </c>
-      <c r="F18" s="46">
+      <c r="F18" s="42">
         <v>0.96</v>
       </c>
-      <c r="G18" s="33"/>
-      <c r="H18" s="46">
+      <c r="G18" s="32"/>
+      <c r="H18" s="42">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I18" s="46">
+      <c r="I18" s="42">
         <v>0.94</v>
       </c>
-      <c r="J18" s="33"/>
-      <c r="K18" s="33">
+      <c r="J18" s="32"/>
+      <c r="K18" s="32">
         <v>0.01</v>
       </c>
-      <c r="L18" s="33">
+      <c r="L18" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
+      <c r="A19" s="25">
         <v>3</v>
       </c>
-      <c r="B19" s="33">
+      <c r="B19" s="32">
         <v>0.09</v>
       </c>
-      <c r="C19" s="33">
+      <c r="C19" s="32">
         <v>0.96</v>
       </c>
-      <c r="D19" s="33"/>
-      <c r="E19" s="46">
+      <c r="D19" s="32"/>
+      <c r="E19" s="42">
         <v>0.21</v>
       </c>
-      <c r="F19" s="46">
+      <c r="F19" s="42">
         <v>0.91</v>
       </c>
-      <c r="G19" s="33"/>
-      <c r="H19" s="46">
+      <c r="G19" s="32"/>
+      <c r="H19" s="42">
         <v>0.12</v>
       </c>
-      <c r="I19" s="46">
+      <c r="I19" s="42">
         <v>0.96</v>
       </c>
-      <c r="J19" s="33"/>
-      <c r="K19" s="33">
+      <c r="J19" s="32"/>
+      <c r="K19" s="32">
         <v>-0.02</v>
       </c>
-      <c r="L19" s="33">
+      <c r="L19" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="31">
         <v>0.09</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="40">
         <v>0.96</v>
       </c>
-      <c r="D20" s="32"/>
-      <c r="E20" s="32">
+      <c r="D20" s="31"/>
+      <c r="E20" s="31">
         <v>0.03</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="40">
         <v>0.97</v>
       </c>
-      <c r="G20" s="32"/>
-      <c r="H20" s="44">
+      <c r="G20" s="31"/>
+      <c r="H20" s="40">
         <v>0.09</v>
       </c>
-      <c r="I20" s="44">
+      <c r="I20" s="40">
         <v>0.96</v>
       </c>
-      <c r="J20" s="32"/>
-      <c r="K20" s="44">
+      <c r="J20" s="31"/>
+      <c r="K20" s="40">
         <v>0.09</v>
       </c>
-      <c r="L20" s="44">
+      <c r="L20" s="40">
         <v>0.95</v>
       </c>
     </row>
@@ -3795,58 +3970,58 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" style="29" customWidth="1"/>
-    <col min="2" max="3" width="20.85546875" style="29" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="29"/>
+    <col min="1" max="1" width="15.28515625" style="28" customWidth="1"/>
+    <col min="2" max="3" width="20.85546875" style="28" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="67" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
     </row>
     <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B2" s="51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="51" t="s">
+      <c r="B2" s="47" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="47" t="s">
         <v>118</v>
       </c>
-      <c r="E2" s="29" t="s">
-        <v>121</v>
+      <c r="E2" s="28" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="49"/>
-      <c r="C3" s="49"/>
+      <c r="B3" s="45"/>
+      <c r="C3" s="45"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="28" t="s">
+      <c r="A5" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
@@ -3857,25 +4032,25 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
+      <c r="B6" s="29"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -3886,25 +4061,25 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
+      <c r="A9" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="52"/>
-      <c r="C9" s="52"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="48"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="29" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="27" t="s">
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
@@ -3915,10 +4090,223 @@
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="48"/>
+      <c r="A21" s="44"/>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="48"/>
+      <c r="A23" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="37.28515625" style="58" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" style="58" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="58" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="58"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="65" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="65" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="65" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="61" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="60"/>
+      <c r="E3" s="60"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+    </row>
+    <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="62" t="s">
+        <v>137</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>127</v>
+      </c>
+      <c r="C5" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5" s="60"/>
+      <c r="E5" s="60"/>
+    </row>
+    <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="62" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>126</v>
+      </c>
+      <c r="D6" s="60"/>
+      <c r="E6" s="60"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="66" t="s">
+        <v>128</v>
+      </c>
+      <c r="B7" s="65" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" s="65" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="60"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="60"/>
+      <c r="E9" s="60"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="62" t="s">
+        <v>134</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>133</v>
+      </c>
+      <c r="C10" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
+        <v>135</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="C11" s="59" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="60"/>
+      <c r="E11" s="60"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="65" t="s">
+        <v>133</v>
+      </c>
+      <c r="C12" s="65" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" s="60"/>
+      <c r="E12" s="60"/>
+    </row>
+    <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="60" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13" s="60"/>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+    </row>
+    <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="60" t="s">
+        <v>140</v>
+      </c>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="60"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="60"/>
+      <c r="E15" s="60"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="60"/>
+      <c r="B16" s="60"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="60"/>
+      <c r="B17" s="60"/>
+      <c r="C17" s="60"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="60"/>
+      <c r="B18" s="60"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
proof before redux resubmit
</commit_message>
<xml_diff>
--- a/word/Tables.xlsx
+++ b/word/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -381,9 +381,6 @@
     </r>
   </si>
   <si>
-    <t>TABLE 1: Summary characteristics of monitoring stations on the Patuxent River estuary. Chlorophyll and salinity  values are based on averages from 1986 to 2014. Stations used for the analysis are in bold. Segments are salinity  regions in the Patuxent for the larger Chesapeake Bay area (TF = tidal fresh, OH = oligohaline, MH = mesohaline). See Figure 1 for site locations.</t>
-  </si>
-  <si>
     <r>
       <t>TABLE 2: Summaries of model performance using RMSE of observed to predicted ln-chl-</t>
     </r>
@@ -1075,13 +1072,36 @@
   </si>
   <si>
     <t>TABLE 8: Qualitative comparisons of generalized additive models and WRTDS. Qualities are grouped by ease of use and statistical considerations. Ease of use qualities are described as good, moderate, or poor and statistical qualities as yes/no.</t>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 1: Summary characteristics of monitoring stations on the Patuxent River estuary. Chlorophyll-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and salinity  values are based on averages from 1986 to 2014. Stations used for the analysis are in bold. Segments are salinity  regions in the Patuxent for the larger Chesapeake Bay area (TF = tidal fresh, OH = oligohaline, MH = mesohaline). See Figure 1 for site locations.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1176,6 +1196,12 @@
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1710,8 +1736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1728,7 +1754,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>109</v>
+        <v>141</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2052,7 +2078,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2393,7 +2419,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2736,7 +2762,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3072,7 +3098,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3412,7 +3438,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3453,31 +3479,31 @@
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="38" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="38" t="s">
+        <v>111</v>
+      </c>
+      <c r="F3" s="38" t="s">
         <v>112</v>
-      </c>
-      <c r="F3" s="38" t="s">
-        <v>113</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="I3" s="38" t="s">
         <v>114</v>
-      </c>
-      <c r="I3" s="38" t="s">
-        <v>115</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="38" t="s">
         <v>114</v>
-      </c>
-      <c r="L3" s="38" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3983,7 +4009,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3993,13 +4019,13 @@
         <v>94</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -4108,7 +4134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4122,14 +4148,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B2" s="65" t="s">
         <v>21</v>
@@ -4142,7 +4168,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -4151,59 +4177,59 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="59" t="s">
+      <c r="C4" s="59" t="s">
         <v>126</v>
-      </c>
-      <c r="C4" s="59" t="s">
-        <v>127</v>
       </c>
       <c r="D4" s="60"/>
       <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="65" t="s">
         <v>128</v>
       </c>
-      <c r="B7" s="65" t="s">
-        <v>129</v>
-      </c>
       <c r="C7" s="65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="60"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -4212,59 +4238,59 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
+        <v>130</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="C9" s="59" t="s">
         <v>132</v>
-      </c>
-      <c r="C9" s="59" t="s">
-        <v>133</v>
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D10" s="60"/>
       <c r="E10" s="60"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D11" s="60"/>
       <c r="E11" s="60"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D12" s="60"/>
       <c r="E12" s="60"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B13" s="60"/>
       <c r="C13" s="60"/>
@@ -4273,7 +4299,7 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="60"/>

</xml_diff>

<commit_message>
revisions up to last general comment done
</commit_message>
<xml_diff>
--- a/word/Tables.xlsx
+++ b/word/Tables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19905" windowHeight="10260" firstSheet="2" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -312,9 +312,6 @@
     <t>Ave. diff.</t>
   </si>
   <si>
-    <t>RMSE</t>
-  </si>
-  <si>
     <t>Simulations</t>
   </si>
   <si>
@@ -378,53 +375,6 @@
         <family val="1"/>
       </rPr>
       <t>g/L )</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 2: Summaries of model performance using RMSE of observed to predicted ln-chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>for each station (LE1.2 and TF1.6). Deviance for each model as the sum of squared residuals is shown in parentheses. Overall performance for the entire time series is shown at the top with groupings by different time periods below. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 5: Comparison of predicted results between WRTDS and GAMs using average differences (%) and RMSE values at each station. Overall comparisons for the entire time series are shown at the top with groupings by different time periods below. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge. Negative percentages indicate WRTDS predictions were lower than GAM predictions (eq. (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF231F20"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>)).</t>
     </r>
   </si>
   <si>
@@ -533,155 +483,7 @@
   </si>
   <si>
     <r>
-      <t>TABLE 6: Regression fits comparing predicted (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>pred</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>) and flow-normalized (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>norm</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>) results for WRTDS and GAMs at each station. Values in bold-italic are those where the intercept (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>β</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>) estimate was significantly different from zero or the slope (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>β</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">) estimate was significantly different from one. Fits for the entire time series are shown at the top. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge. See Figure </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF231F20"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">5 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>for a graphical  summary.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 7: Summaries of model performance comparing observed chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>with predicted values (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>Chl</t>
+      <t>C hl</t>
     </r>
     <r>
       <rPr>
@@ -692,7 +494,7 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>obs</t>
+      <t>bio</t>
     </r>
     <r>
       <rPr>
@@ -713,44 +515,14 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>obs</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>) and biological chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> with flow-normalized  values (</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
+      <t>bio</t>
+    </r>
+  </si>
+  <si>
+    <t>Add hats to second chl text in each formula</t>
+  </si>
+  <si>
+    <r>
       <t>Chl</t>
     </r>
     <r>
@@ -760,9 +532,8 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>bio</t>
+      </rPr>
+      <t>obs</t>
     </r>
     <r>
       <rPr>
@@ -781,23 +552,398 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>bio</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>) for the three simulated time series (no flow, constant flow, and increasing flow effect). Summaries are RMSE values comparing results from each model (GAM, WRTDS).  Deviance for each model as the sum of squared residuals is shown in parentheses.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>C hl</t>
+      </rPr>
+      <t>obs</t>
+    </r>
+  </si>
+  <si>
+    <t>Quality</t>
+  </si>
+  <si>
+    <t>ease of use</t>
+  </si>
+  <si>
+    <t>computational requirements</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>visualization</t>
+  </si>
+  <si>
+    <t>moderate</t>
+  </si>
+  <si>
+    <t>statistical</t>
+  </si>
+  <si>
+    <t>additional variables</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>censored data</t>
+  </si>
+  <si>
+    <t>confidence intervals</t>
+  </si>
+  <si>
+    <t>quantile fits</t>
+  </si>
+  <si>
+    <r>
+      <t>interpretation</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>software and documentation</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Relates to statistical foundation</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>In reference to analysis of water quality trends</t>
+    </r>
+  </si>
+  <si>
+    <t>TABLE 8: Qualitative comparisons of generalized additive models and WRTDS. Qualities are grouped by ease of use and statistical considerations. Ease of use qualities are described as good, moderate, or poor and statistical qualities as yes/no.</t>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 1: Summary characteristics of monitoring stations on the Patuxent River estuary. Chlorophyll-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+      </rPr>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> and salinity  values are based on averages from 1986 to 2014. Stations used for the analysis are in bold. Segments are salinity  regions in the Patuxent for the larger Chesapeake Bay area (TF = tidal fresh, OH = oligohaline, MH = mesohaline).</t>
+    </r>
+  </si>
+  <si>
+    <t>TABLE 2: Summaries of model performance using RMSE (deviance in parentheses) of observed to predicted ln-chl-a for each station (LE1.2 and TF1.6). Overall performance for the entire time series is shown at the top with groupings by different time periods below. Time periods are annual groupings every seven years (top), seasonal groupings (middle), and flow periods based on quantile distributions of discharge.</t>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 3: Summaries of flow-normalized trends from each model at LE1.2 for different time periods. Summaries are averages and percentage changes of ln-chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>g/L) based on annual means within each category. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings (middle), and flow periods based on quantile distributions of discharge.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 4: Summaries of flow-normalized  trends from each model  at TF1.6 for different time periods. Summaries  are averages and percentage changes of ln-chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>g/L ) based on annual means within each category. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings (middle), and flow periods based on quantile distributions of discharge.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 5: Comparison of predicted results between WRTDS and GAMs using average differences (%) and RMSD. Overall comparisons for the entire time series are shown at the top with groupings by different time periods below. Time periods are annual groupings every seven years (top), seasonal groupings (middle), and flow periods based on quantile distributions of discharge. Negative percentages indicate WRTDS predictions were lower than GAM predictions (eq. (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF231F20"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>)).</t>
+    </r>
+  </si>
+  <si>
+    <t>RMSD</t>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 6: Regression fits comparing predicted (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>pred</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) and flow-normalized (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>norm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) results for WRTDS and GAMs. Values in bold-italic are those where the intercept (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) estimate was significantly different from zero or the slope (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>β</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) estimate was significantly different from one. Fits for the entire time series are shown at the top. Time periods are annual groupings every seven years (top), seasonal groupings (middle), and flow periods based on quantile distributions of discharge.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>TABLE 7: Summaries of model performance comparing observed chl-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>with predicted values (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>Chl</t>
     </r>
     <r>
       <rPr>
@@ -808,7 +954,7 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>bio</t>
+      <t>obs</t>
     </r>
     <r>
       <rPr>
@@ -829,12 +975,16 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>bio</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 4: Summaries of flow-normalized  trends from each model  at TF1.6 for different time periods. Summaries  are averages and percentage changes of ln-chl-</t>
+      <t>obs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) and biological chl-</t>
     </r>
     <r>
       <rPr>
@@ -844,16 +994,16 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
+      <t>a</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> with flow-normalized  values (</t>
     </r>
     <r>
       <rPr>
@@ -863,66 +1013,6 @@
         <rFont val="Times"/>
         <family val="1"/>
       </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>g/L ) based on annual means within each category.  For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
-    </r>
-  </si>
-  <si>
-    <t>Add hats to second chl text in each formula</t>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 3: Summaries of flow-normalized trends from each model at LE1.2 for different time periods. Summaries are averages and percentage changes of ln-chl-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>(</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>µ</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t>g/L) based on annual means within each category. For example, summary values for high flow for a given model are based on instances of high flow across years. Percentage changes are the differences  between the last and first years in the periods. Time periods are annual groupings every seven years (top), seasonal groupings by monthly quarters (middle), and flow periods based on quantile distributions of discharge.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>Chl</t>
     </r>
     <r>
@@ -932,8 +1022,9 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-      </rPr>
-      <t>obs</t>
+        <family val="1"/>
+      </rPr>
+      <t>bio</t>
     </r>
     <r>
       <rPr>
@@ -952,148 +1043,18 @@
         <sz val="12"/>
         <color theme="1"/>
         <rFont val="Times"/>
-      </rPr>
-      <t>obs</t>
-    </r>
-  </si>
-  <si>
-    <t>Quality</t>
-  </si>
-  <si>
-    <t>ease of use</t>
-  </si>
-  <si>
-    <t>computational requirements</t>
-  </si>
-  <si>
-    <t>good</t>
-  </si>
-  <si>
-    <t>poor</t>
-  </si>
-  <si>
-    <t>visualization</t>
-  </si>
-  <si>
-    <t>moderate</t>
-  </si>
-  <si>
-    <t>statistical</t>
-  </si>
-  <si>
-    <t>additional variables</t>
-  </si>
-  <si>
-    <t>y</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>censored data</t>
-  </si>
-  <si>
-    <t>confidence intervals</t>
-  </si>
-  <si>
-    <t>quantile fits</t>
-  </si>
-  <si>
-    <r>
-      <t>interpretation</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>software and documentation</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Relates to statistical foundation</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>In reference to analysis of water quality trends</t>
-    </r>
-  </si>
-  <si>
-    <t>TABLE 8: Qualitative comparisons of generalized additive models and WRTDS. Qualities are grouped by ease of use and statistical considerations. Ease of use qualities are described as good, moderate, or poor and statistical qualities as yes/no.</t>
-  </si>
-  <si>
-    <r>
-      <t>TABLE 1: Summary characteristics of monitoring stations on the Patuxent River estuary. Chlorophyll-</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-      </rPr>
-      <t>a</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> and salinity  values are based on averages from 1986 to 2014. Stations used for the analysis are in bold. Segments are salinity  regions in the Patuxent for the larger Chesapeake Bay area (TF = tidal fresh, OH = oligohaline, MH = mesohaline). See Figure 1 for site locations.</t>
+        <family val="1"/>
+      </rPr>
+      <t>bio</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times"/>
+        <family val="1"/>
+      </rPr>
+      <t>) for the three simulated time series (no flow, constant flow, and increasing flow effect). Summaries are RMSE values (deviance in parentheses) comparing results from each model (GAM, WRTDS).</t>
     </r>
   </si>
 </sst>
@@ -1736,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1752,9 +1713,9 @@
     <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -1784,7 +1745,7 @@
         <v>5</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H2" s="8" t="s">
         <v>6</v>
@@ -2063,8 +2024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2078,7 +2039,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>109</v>
+        <v>135</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2403,7 +2364,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F20"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2417,9 +2378,9 @@
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="126" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>120</v>
+        <v>136</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -2745,8 +2706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F20"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2760,9 +2721,9 @@
     <col min="7" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>118</v>
+        <v>137</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3084,7 +3045,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F20"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3096,9 +3057,9 @@
     <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="129.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="113.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3126,14 +3087,14 @@
         <v>92</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7" t="s">
         <v>92</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -3184,7 +3145,7 @@
       </c>
       <c r="D7" s="32"/>
       <c r="E7" s="32">
-        <v>-0.74</v>
+        <v>-0.75</v>
       </c>
       <c r="F7" s="32">
         <v>0.11</v>
@@ -3238,7 +3199,7 @@
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31">
-        <v>3.1</v>
+        <v>3.06</v>
       </c>
       <c r="F10" s="31">
         <v>0.14000000000000001</v>
@@ -3266,7 +3227,7 @@
       </c>
       <c r="D12" s="34"/>
       <c r="E12" s="32">
-        <v>-2</v>
+        <v>-2.02</v>
       </c>
       <c r="F12" s="32">
         <v>0.14000000000000001</v>
@@ -3320,7 +3281,7 @@
       </c>
       <c r="D15" s="31"/>
       <c r="E15" s="31">
-        <v>1.04</v>
+        <v>1.03</v>
       </c>
       <c r="F15" s="31">
         <v>0.15</v>
@@ -3377,14 +3338,14 @@
         <v>3</v>
       </c>
       <c r="B19" s="32">
-        <v>0.49</v>
+        <v>0.48</v>
       </c>
       <c r="C19" s="32">
         <v>0.11</v>
       </c>
       <c r="D19" s="32"/>
       <c r="E19" s="32">
-        <v>1.07</v>
+        <v>1.06</v>
       </c>
       <c r="F19" s="32">
         <v>0.14000000000000001</v>
@@ -3402,7 +3363,7 @@
       </c>
       <c r="D20" s="31"/>
       <c r="E20" s="31">
-        <v>-1.75</v>
+        <v>-1.77</v>
       </c>
       <c r="F20" s="31">
         <v>0.15</v>
@@ -3421,7 +3382,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:L20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3436,9 +3397,9 @@
     <col min="11" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="87" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>115</v>
+        <v>140</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
@@ -3479,31 +3440,31 @@
     <row r="3" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
       <c r="B3" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="F3" s="38" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G3" s="6"/>
       <c r="H3" s="38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="I3" s="38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="J3" s="6"/>
       <c r="K3" s="38" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="L3" s="38" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -3997,7 +3958,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4009,28 +3970,28 @@
   <sheetData>
     <row r="1" spans="1:5" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="67" t="s">
-        <v>116</v>
+        <v>141</v>
       </c>
       <c r="B1" s="67"/>
       <c r="C1" s="67"/>
     </row>
     <row r="2" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C2" s="47" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E2" s="28" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="45"/>
       <c r="C3" s="45"/>
@@ -4040,10 +4001,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>96</v>
-      </c>
-      <c r="C4" s="29" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -4051,15 +4012,15 @@
         <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>98</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
@@ -4069,10 +4030,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -4080,15 +4041,15 @@
         <v>22</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>102</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B9" s="48"/>
       <c r="C9" s="48"/>
@@ -4098,10 +4059,10 @@
         <v>21</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -4109,10 +4070,10 @@
         <v>22</v>
       </c>
       <c r="B11" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -4134,7 +4095,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -4148,14 +4109,14 @@
   <sheetData>
     <row r="1" spans="1:5" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="B1" s="71"/>
       <c r="C1" s="71"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="65" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B2" s="65" t="s">
         <v>21</v>
@@ -4168,7 +4129,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="61" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B3" s="59"/>
       <c r="C3" s="59"/>
@@ -4177,59 +4138,59 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B4" s="59" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D4" s="60"/>
       <c r="E4" s="60"/>
     </row>
     <row r="5" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B5" s="59" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D5" s="60"/>
       <c r="E5" s="60"/>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="62" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D6" s="60"/>
       <c r="E6" s="60"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="66" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B7" s="65" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C7" s="65" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D7" s="60"/>
       <c r="E7" s="60"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="64" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -4238,59 +4199,59 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="62" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="D9" s="60"/>
       <c r="E9" s="60"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="62" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C10" s="59" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D10" s="60"/>
       <c r="E10" s="60"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="62" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B11" s="59" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C11" s="59" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D11" s="60"/>
       <c r="E11" s="60"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="66" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B12" s="65" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C12" s="65" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D12" s="60"/>
       <c r="E12" s="60"/>
     </row>
     <row r="13" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="60" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B13" s="60"/>
       <c r="C13" s="60"/>
@@ -4299,7 +4260,7 @@
     </row>
     <row r="14" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="60" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="B14" s="60"/>
       <c r="C14" s="60"/>

</xml_diff>